<commit_message>
Updated app.py and storage.xlsx
</commit_message>
<xml_diff>
--- a/storage.xlsx
+++ b/storage.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarav\Downloads\model_web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarav\Projects\model_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB679EA1-A0AE-4AD8-A042-1B4444B25327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901189A0-3E37-4A72-9102-4FC3DE48E54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2339942C-4166-42DF-A1C1-2F62199EC0BF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2339942C-4166-42DF-A1C1-2F62199EC0BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blouse" sheetId="1" r:id="rId1"/>
+    <sheet name="Sleeve Designs" sheetId="4" r:id="rId2"/>
+    <sheet name="Neck Designs" sheetId="3" r:id="rId3"/>
+    <sheet name="Aari" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="192">
   <si>
     <t>ID</t>
   </si>
@@ -676,7 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -702,7 +705,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -715,6 +717,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1030,21 +1044,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFCCAB43-1872-4865-89F7-C7A4C5F77C34}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" customWidth="1"/>
-    <col min="7" max="8" width="23.5546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="113.21875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="26.77734375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="4"/>
+    <col min="5" max="8" width="23.5546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="113.21875" style="6" customWidth="1"/>
     <col min="10" max="10" width="29" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1174,87 +1189,87 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>137</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>136</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>138</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>138</v>
+        <v>9</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2">
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>118</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>120</v>
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="58.2" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>126</v>
+      <c r="B7" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2">
-        <v>2000</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>128</v>
+        <v>300</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>128</v>
+        <v>9</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="6" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -1262,84 +1277,80 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>125</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2">
-        <v>1000</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>129</v>
+        <v>400</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>129</v>
+        <v>9</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="D9" s="2">
-        <v>150</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>174</v>
+        <v>400</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>175</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>142</v>
+        <v>82</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2">
-        <v>100</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>176</v>
+        <v>300</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>177</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="3"/>
       <c r="I10" s="6" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -1347,28 +1358,26 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>135</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2">
-        <v>150</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>178</v>
+        <v>400</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>179</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="3"/>
       <c r="I11" s="6" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -1376,26 +1385,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="3"/>
+        <v>13</v>
+      </c>
       <c r="I12" s="6" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -1403,82 +1411,83 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2">
         <v>400</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="3"/>
+        <v>44</v>
+      </c>
       <c r="I14" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D15" s="2">
         <v>400</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="I15" s="6" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -1486,577 +1495,164 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D16" s="2">
         <v>400</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="I16" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>82</v>
+      <c r="B17" s="10" t="s">
+        <v>99</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="D17" s="2">
-        <v>300</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>37</v>
+        <v>400</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="3"/>
+      <c r="G17" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="I17" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>84</v>
+      <c r="B18" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="D18" s="2">
         <v>400</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>38</v>
+      <c r="E18" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="3"/>
+      <c r="G18" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="I18" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>86</v>
+      <c r="B19" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="D19" s="2">
         <v>400</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>14</v>
+      <c r="E19" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>13</v>
+      <c r="G19" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>88</v>
+      <c r="B20" s="10" t="s">
+        <v>113</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="D20" s="2">
         <v>400</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>40</v>
+      <c r="E20" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="2">
-        <v>400</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="2">
-        <v>400</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="2">
-        <v>400</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="2">
-        <v>400</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="2">
-        <v>400</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" s="2">
-        <v>400</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
-        <v>26</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D27" s="2">
-        <v>400</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H20" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I20" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="2">
-        <v>150</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>180</v>
-      </c>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="5"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
-        <v>28</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D29" s="2">
-        <v>150</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D30" s="2">
-        <v>200</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="F30" t="s">
-        <v>152</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D31" s="2">
-        <v>200</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="F31" t="s">
-        <v>152</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.35">
-      <c r="A32" s="2">
-        <v>31</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D32" s="2">
-        <v>200</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="F32" t="s">
-        <v>152</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
-        <v>32</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D33" s="2">
-        <v>200</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="F33" t="s">
-        <v>152</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="75" x14ac:dyDescent="0.35">
-      <c r="A34" s="2">
-        <v>33</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D34" s="2">
-        <v>200</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="F34" t="s">
-        <v>152</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.35">
-      <c r="A35" s="2">
-        <v>34</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D35" s="2">
-        <v>200</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="F35" t="s">
-        <v>152</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>35</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D36" s="2">
-        <v>1000</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="F36" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>173</v>
-      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2064,91 +1660,699 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{FB588CA0-8FE0-4EE5-B29B-97C29D8D516F}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{23654C75-5E67-4C24-983D-BB2A72E63E63}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{3CD6EC97-8052-4EC4-A249-60D56D2A1313}"/>
-    <hyperlink ref="E16" r:id="rId4" xr:uid="{15DC04D7-577A-4E97-A7F0-D9DA3ECC3FF8}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{15DC04D7-577A-4E97-A7F0-D9DA3ECC3FF8}"/>
     <hyperlink ref="G2" r:id="rId5" xr:uid="{2609FC5E-AF31-468F-934A-62A90286B25D}"/>
     <hyperlink ref="G3" r:id="rId6" xr:uid="{DBB8975B-8131-4CDD-937C-D2E6119FE7E1}"/>
     <hyperlink ref="G4" r:id="rId7" xr:uid="{76AF5CAD-364C-45A5-86DC-D2E6819F8F0D}"/>
     <hyperlink ref="H2" r:id="rId8" xr:uid="{89AB311D-122A-4B19-91A1-A164EC864B0B}"/>
     <hyperlink ref="H3" r:id="rId9" xr:uid="{4B8CA1F4-97B0-472E-BEB5-B5622FDE9A8C}"/>
     <hyperlink ref="J2" r:id="rId10" xr:uid="{6ABD0D54-B22E-4D4C-B4E8-CFC1B253AD0F}"/>
-    <hyperlink ref="G19" r:id="rId11" xr:uid="{45C9AE52-071E-4962-8D20-95F034984604}"/>
-    <hyperlink ref="E19" r:id="rId12" xr:uid="{BAB9B680-A9F2-4691-92AB-8CA16333E586}"/>
+    <hyperlink ref="G12" r:id="rId11" xr:uid="{45C9AE52-071E-4962-8D20-95F034984604}"/>
+    <hyperlink ref="E12" r:id="rId12" xr:uid="{BAB9B680-A9F2-4691-92AB-8CA16333E586}"/>
     <hyperlink ref="J3" r:id="rId13" xr:uid="{454457E2-A2B4-45A6-8CAC-F706047944DC}"/>
-    <hyperlink ref="E12" r:id="rId14" xr:uid="{5CC2990D-BC12-45A2-83E7-B03684EE886E}"/>
-    <hyperlink ref="G12" r:id="rId15" xr:uid="{8CFEFD14-3664-47EE-BC80-B298F50237A9}"/>
-    <hyperlink ref="E13" r:id="rId16" xr:uid="{2D5BBA18-92F2-40BB-9EB8-EFD87F9D001C}"/>
-    <hyperlink ref="G13" r:id="rId17" xr:uid="{3656CA5F-A78A-4454-A2F6-9FEEF8954739}"/>
-    <hyperlink ref="H13" r:id="rId18" xr:uid="{12364E9F-310A-4356-96F6-C2D4EAD0BA46}"/>
-    <hyperlink ref="E14" r:id="rId19" xr:uid="{A29E35D1-5557-4DAF-A2FB-4A9DA16C0CBB}"/>
-    <hyperlink ref="G14" r:id="rId20" xr:uid="{5B8AECDC-1B9F-492D-89F2-183CCCD0EFD0}"/>
-    <hyperlink ref="E15" r:id="rId21" xr:uid="{2918C589-AF11-4E89-AE18-FF2D7AE19B4B}"/>
-    <hyperlink ref="G15" r:id="rId22" xr:uid="{F4E5B8C2-9C48-419D-97A9-26337B53DF6D}"/>
-    <hyperlink ref="G16" r:id="rId23" xr:uid="{4E464582-FFB0-4793-9714-C58235BF6745}"/>
-    <hyperlink ref="G17" r:id="rId24" xr:uid="{3C2446F1-D51F-465B-848C-0C35F1367F32}"/>
-    <hyperlink ref="E17" r:id="rId25" xr:uid="{3D11D4E4-02E9-4B61-9D19-60AF15169DDB}"/>
-    <hyperlink ref="E18" r:id="rId26" xr:uid="{CF25CD4A-927D-4AA4-823B-89DC9DB5FFA4}"/>
-    <hyperlink ref="G18" r:id="rId27" xr:uid="{B4266B19-0026-4D82-A603-4C8A8F004CD0}"/>
-    <hyperlink ref="E20" r:id="rId28" xr:uid="{974BB6BD-8D12-44F8-BD25-ED3B023AA159}"/>
-    <hyperlink ref="G20" r:id="rId29" xr:uid="{89486677-3D0A-4727-AAB8-50B053538F64}"/>
-    <hyperlink ref="H20" r:id="rId30" xr:uid="{552349D2-7A6B-494F-843F-B331DBB1B6DE}"/>
-    <hyperlink ref="E21" r:id="rId31" xr:uid="{2D8CF422-AED1-4872-87A8-B3AE516D92EF}"/>
-    <hyperlink ref="G21" r:id="rId32" xr:uid="{1DEDB661-7442-4A5C-A6F7-1204C9F7868D}"/>
-    <hyperlink ref="E22" r:id="rId33" xr:uid="{B8A5B01A-5E9E-40D2-B571-ADDB1A198C99}"/>
-    <hyperlink ref="G22" r:id="rId34" xr:uid="{4DD77962-FBE1-4859-B50B-D5E413F68A58}"/>
-    <hyperlink ref="H22" r:id="rId35" xr:uid="{6CF5B222-9B1A-49B5-8683-69291053DB5F}"/>
-    <hyperlink ref="E23" r:id="rId36" xr:uid="{31170597-1143-45DA-8EEC-EC904E2AFA08}"/>
-    <hyperlink ref="G23" r:id="rId37" xr:uid="{CED90838-C76F-44A4-A2C5-09269BBC4655}"/>
-    <hyperlink ref="H23" r:id="rId38" xr:uid="{87B5E26B-DD33-4BD3-8D07-A7B945B3D571}"/>
-    <hyperlink ref="E24" r:id="rId39" xr:uid="{E05D18F5-751E-4091-B123-91A57C520FC6}"/>
-    <hyperlink ref="G24" r:id="rId40" xr:uid="{E03ABA7C-2372-4F36-99A0-19793C991FE9}"/>
-    <hyperlink ref="H24" r:id="rId41" xr:uid="{3047CBCC-C689-42A1-8D72-9274A6FDC822}"/>
-    <hyperlink ref="E25" r:id="rId42" xr:uid="{ED800B34-310D-4333-87B4-7F8A28AF7281}"/>
-    <hyperlink ref="G25" r:id="rId43" xr:uid="{693D6087-C936-426F-9B04-9C370F655F31}"/>
-    <hyperlink ref="E26" r:id="rId44" xr:uid="{D9C01FB5-466F-41F0-9D38-9704569EA9E5}"/>
-    <hyperlink ref="G26" r:id="rId45" xr:uid="{35D34652-F90D-4C3A-910E-3B3A70FF9D06}"/>
-    <hyperlink ref="H26" r:id="rId46" xr:uid="{01393D58-137F-4AA2-BE58-17C5803F82A8}"/>
-    <hyperlink ref="E27" r:id="rId47" xr:uid="{E39D3659-8C1C-4C0D-9144-A38D783327CD}"/>
-    <hyperlink ref="G27" r:id="rId48" xr:uid="{6D8DB014-4EF3-4F4D-B951-2611CC01F94D}"/>
-    <hyperlink ref="H27" r:id="rId49" xr:uid="{3C91ECEE-FA8D-4E90-B1E5-88EA592CDA5C}"/>
-    <hyperlink ref="E6" r:id="rId50" xr:uid="{6FE1A839-3A66-40C7-9D47-E837FA302749}"/>
-    <hyperlink ref="G6" r:id="rId51" xr:uid="{8A7CA079-BFEC-49EB-83DB-DFA7EAC9D464}"/>
-    <hyperlink ref="H6" r:id="rId52" xr:uid="{EABF28BA-3446-41C0-A651-84262A2A5CB4}"/>
-    <hyperlink ref="E7" r:id="rId53" xr:uid="{50A935C9-6BD0-41D8-AF96-33ECC98CFCC2}"/>
-    <hyperlink ref="G7" r:id="rId54" xr:uid="{5C0858DE-B83F-44B8-B658-10382FDE2DB0}"/>
-    <hyperlink ref="E8" r:id="rId55" xr:uid="{EA14F21F-B7F6-49B9-A1BF-953234F55846}"/>
-    <hyperlink ref="G8" r:id="rId56" xr:uid="{906B007D-FB38-4944-83F9-55524AFCE3C3}"/>
-    <hyperlink ref="E5" r:id="rId57" xr:uid="{22867B7B-755D-4F5B-A810-CABC89F0523E}"/>
-    <hyperlink ref="G5" r:id="rId58" xr:uid="{145D8C38-9220-4A76-9285-65B341DC99A8}"/>
-    <hyperlink ref="E9" r:id="rId59" xr:uid="{81CB0DE7-37A5-41AC-8B9D-28FC70AA6128}"/>
-    <hyperlink ref="G9" r:id="rId60" xr:uid="{D9A6E10D-3996-434A-B16F-1A65493E1798}"/>
-    <hyperlink ref="H9" r:id="rId61" xr:uid="{F0E5610F-332A-4DA7-B0FB-2518E730EC36}"/>
-    <hyperlink ref="E10" r:id="rId62" xr:uid="{9F54F99E-2603-4BEC-8227-A2099A701C34}"/>
-    <hyperlink ref="G10" r:id="rId63" xr:uid="{8CFBC6B5-986F-4323-A0B5-99B1124367E9}"/>
-    <hyperlink ref="H10" r:id="rId64" xr:uid="{8C1360BC-BE58-458A-827A-22D86C38B38E}"/>
-    <hyperlink ref="E11" r:id="rId65" xr:uid="{A3280345-512D-49C6-BDC8-4F1788F70215}"/>
-    <hyperlink ref="G11" r:id="rId66" xr:uid="{0672CF34-0557-4BB2-9459-C01E74D6065D}"/>
-    <hyperlink ref="H11" r:id="rId67" xr:uid="{B5FACE55-7AA8-45DD-B368-9EEE99A4A9CD}"/>
-    <hyperlink ref="E28" r:id="rId68" xr:uid="{85093D72-C26A-4119-9269-5E41B93BE190}"/>
-    <hyperlink ref="G28" r:id="rId69" xr:uid="{E580AC50-9D07-4547-B199-617DF801F6D0}"/>
-    <hyperlink ref="E29" r:id="rId70" xr:uid="{E1D411ED-DC55-46A4-9016-724CDA5F7835}"/>
-    <hyperlink ref="G29" r:id="rId71" xr:uid="{E4494067-FDD7-4ACB-B2A6-91B19BCEA5FB}"/>
-    <hyperlink ref="H29" r:id="rId72" xr:uid="{A371C7C7-D292-465D-84F0-75185ADB763A}"/>
-    <hyperlink ref="J29" r:id="rId73" xr:uid="{0FEDD489-D710-4EA8-8E23-69BEFE39A64E}"/>
-    <hyperlink ref="E30" r:id="rId74" xr:uid="{D0165883-B711-4AE6-B3D2-78B807C6FEA0}"/>
-    <hyperlink ref="G30" r:id="rId75" xr:uid="{137FBA2D-574D-4B81-80EA-917919005AE4}"/>
-    <hyperlink ref="E31" r:id="rId76" xr:uid="{0BC74270-8F34-4D4E-B265-83C3F4046B28}"/>
-    <hyperlink ref="G31" r:id="rId77" xr:uid="{49F47022-8407-4DC7-9878-C0EBB909F052}"/>
-    <hyperlink ref="H31" r:id="rId78" xr:uid="{51E5E6E3-F3E7-4AAF-A1E9-16B2C2EBC272}"/>
-    <hyperlink ref="E32" r:id="rId79" xr:uid="{EC92CBA8-9711-476A-8514-A46970AB4330}"/>
-    <hyperlink ref="G32" r:id="rId80" xr:uid="{9A65B6E6-CE9F-46BD-A8CB-5883912994BF}"/>
-    <hyperlink ref="E33" r:id="rId81" xr:uid="{DA0F76FF-E012-45EB-BDEC-0702B556D5D6}"/>
-    <hyperlink ref="G33" r:id="rId82" xr:uid="{B44C7F1E-5837-4FBE-A45D-CE69E94A8743}"/>
-    <hyperlink ref="E34" r:id="rId83" xr:uid="{48486199-52A3-4233-B9B3-FCF585AD9015}"/>
-    <hyperlink ref="G34" r:id="rId84" xr:uid="{E416AE9F-9A48-4AC3-B097-BE2D814BB3ED}"/>
-    <hyperlink ref="E35" r:id="rId85" xr:uid="{37215E58-29AD-443E-A4E9-484E5B03594F}"/>
-    <hyperlink ref="G35" r:id="rId86" xr:uid="{D57B77ED-066E-4D97-AECD-EBFF50C0E174}"/>
-    <hyperlink ref="E36" r:id="rId87" xr:uid="{B086BF29-0CA6-41D0-AFCE-7673ED72DDAE}"/>
-    <hyperlink ref="G36" r:id="rId88" xr:uid="{FF0A2560-C670-4D35-9AE8-D4B3471441BE}"/>
+    <hyperlink ref="E5" r:id="rId14" xr:uid="{5CC2990D-BC12-45A2-83E7-B03684EE886E}"/>
+    <hyperlink ref="G5" r:id="rId15" xr:uid="{8CFEFD14-3664-47EE-BC80-B298F50237A9}"/>
+    <hyperlink ref="E6" r:id="rId16" xr:uid="{2D5BBA18-92F2-40BB-9EB8-EFD87F9D001C}"/>
+    <hyperlink ref="G6" r:id="rId17" xr:uid="{3656CA5F-A78A-4454-A2F6-9FEEF8954739}"/>
+    <hyperlink ref="H6" r:id="rId18" xr:uid="{12364E9F-310A-4356-96F6-C2D4EAD0BA46}"/>
+    <hyperlink ref="E7" r:id="rId19" xr:uid="{A29E35D1-5557-4DAF-A2FB-4A9DA16C0CBB}"/>
+    <hyperlink ref="G7" r:id="rId20" xr:uid="{5B8AECDC-1B9F-492D-89F2-183CCCD0EFD0}"/>
+    <hyperlink ref="E8" r:id="rId21" xr:uid="{2918C589-AF11-4E89-AE18-FF2D7AE19B4B}"/>
+    <hyperlink ref="G8" r:id="rId22" xr:uid="{F4E5B8C2-9C48-419D-97A9-26337B53DF6D}"/>
+    <hyperlink ref="G9" r:id="rId23" xr:uid="{4E464582-FFB0-4793-9714-C58235BF6745}"/>
+    <hyperlink ref="G10" r:id="rId24" xr:uid="{3C2446F1-D51F-465B-848C-0C35F1367F32}"/>
+    <hyperlink ref="E10" r:id="rId25" xr:uid="{3D11D4E4-02E9-4B61-9D19-60AF15169DDB}"/>
+    <hyperlink ref="E11" r:id="rId26" xr:uid="{CF25CD4A-927D-4AA4-823B-89DC9DB5FFA4}"/>
+    <hyperlink ref="G11" r:id="rId27" xr:uid="{B4266B19-0026-4D82-A603-4C8A8F004CD0}"/>
+    <hyperlink ref="E13" r:id="rId28" xr:uid="{974BB6BD-8D12-44F8-BD25-ED3B023AA159}"/>
+    <hyperlink ref="G13" r:id="rId29" xr:uid="{89486677-3D0A-4727-AAB8-50B053538F64}"/>
+    <hyperlink ref="H13" r:id="rId30" xr:uid="{552349D2-7A6B-494F-843F-B331DBB1B6DE}"/>
+    <hyperlink ref="E14" r:id="rId31" xr:uid="{2D8CF422-AED1-4872-87A8-B3AE516D92EF}"/>
+    <hyperlink ref="G14" r:id="rId32" xr:uid="{1DEDB661-7442-4A5C-A6F7-1204C9F7868D}"/>
+    <hyperlink ref="E15" r:id="rId33" xr:uid="{B8A5B01A-5E9E-40D2-B571-ADDB1A198C99}"/>
+    <hyperlink ref="G15" r:id="rId34" xr:uid="{4DD77962-FBE1-4859-B50B-D5E413F68A58}"/>
+    <hyperlink ref="H15" r:id="rId35" xr:uid="{6CF5B222-9B1A-49B5-8683-69291053DB5F}"/>
+    <hyperlink ref="E16" r:id="rId36" xr:uid="{31170597-1143-45DA-8EEC-EC904E2AFA08}"/>
+    <hyperlink ref="G16" r:id="rId37" xr:uid="{CED90838-C76F-44A4-A2C5-09269BBC4655}"/>
+    <hyperlink ref="H16" r:id="rId38" xr:uid="{87B5E26B-DD33-4BD3-8D07-A7B945B3D571}"/>
+    <hyperlink ref="E17" r:id="rId39" xr:uid="{E05D18F5-751E-4091-B123-91A57C520FC6}"/>
+    <hyperlink ref="G17" r:id="rId40" xr:uid="{E03ABA7C-2372-4F36-99A0-19793C991FE9}"/>
+    <hyperlink ref="H17" r:id="rId41" xr:uid="{3047CBCC-C689-42A1-8D72-9274A6FDC822}"/>
+    <hyperlink ref="E18" r:id="rId42" xr:uid="{ED800B34-310D-4333-87B4-7F8A28AF7281}"/>
+    <hyperlink ref="G18" r:id="rId43" xr:uid="{693D6087-C936-426F-9B04-9C370F655F31}"/>
+    <hyperlink ref="E19" r:id="rId44" xr:uid="{D9C01FB5-466F-41F0-9D38-9704569EA9E5}"/>
+    <hyperlink ref="G19" r:id="rId45" xr:uid="{35D34652-F90D-4C3A-910E-3B3A70FF9D06}"/>
+    <hyperlink ref="H19" r:id="rId46" xr:uid="{01393D58-137F-4AA2-BE58-17C5803F82A8}"/>
+    <hyperlink ref="E20" r:id="rId47" xr:uid="{E39D3659-8C1C-4C0D-9144-A38D783327CD}"/>
+    <hyperlink ref="G20" r:id="rId48" xr:uid="{6D8DB014-4EF3-4F4D-B951-2611CC01F94D}"/>
+    <hyperlink ref="H20" r:id="rId49" xr:uid="{3C91ECEE-FA8D-4E90-B1E5-88EA592CDA5C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36BFA87-C568-4F4E-8A59-52B3FCE9FFED}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="15"/>
+    <col min="3" max="3" width="19" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="12">
+        <v>150</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="16"/>
+      <c r="I2" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="12">
+        <v>150</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="12">
+        <v>100</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="12">
+        <v>150</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="12">
+        <v>150</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="12">
+        <v>150</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{22867B7B-755D-4F5B-A810-CABC89F0523E}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{145D8C38-9220-4A76-9285-65B341DC99A8}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{81CB0DE7-37A5-41AC-8B9D-28FC70AA6128}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{D9A6E10D-3996-434A-B16F-1A65493E1798}"/>
+    <hyperlink ref="H3" r:id="rId5" xr:uid="{F0E5610F-332A-4DA7-B0FB-2518E730EC36}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{9F54F99E-2603-4BEC-8227-A2099A701C34}"/>
+    <hyperlink ref="G4" r:id="rId7" xr:uid="{8CFBC6B5-986F-4323-A0B5-99B1124367E9}"/>
+    <hyperlink ref="H4" r:id="rId8" xr:uid="{8C1360BC-BE58-458A-827A-22D86C38B38E}"/>
+    <hyperlink ref="E5" r:id="rId9" xr:uid="{A3280345-512D-49C6-BDC8-4F1788F70215}"/>
+    <hyperlink ref="G5" r:id="rId10" xr:uid="{0672CF34-0557-4BB2-9459-C01E74D6065D}"/>
+    <hyperlink ref="H5" r:id="rId11" xr:uid="{B5FACE55-7AA8-45DD-B368-9EEE99A4A9CD}"/>
+    <hyperlink ref="E6" r:id="rId12" xr:uid="{D2987D09-B1EF-44C0-B5AD-66886139BE1B}"/>
+    <hyperlink ref="G6" r:id="rId13" xr:uid="{D99CF6D2-1A24-43BD-94BC-F56553117B27}"/>
+    <hyperlink ref="E7" r:id="rId14" xr:uid="{D48366C3-52EF-43EA-B7DB-38A6A853B1A0}"/>
+    <hyperlink ref="G7" r:id="rId15" xr:uid="{980A975F-A397-4CF4-A71F-545337F14333}"/>
+    <hyperlink ref="H7" r:id="rId16" xr:uid="{266608AC-4519-4F35-A6CE-66CA58EF2A18}"/>
+    <hyperlink ref="J7" r:id="rId17" xr:uid="{DC3423A7-31F6-4F7A-98CF-EB74179DF769}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9A80E3-8885-447B-B2AB-3DD175D4CA0B}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="12">
+        <v>200</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="12">
+        <v>200</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="12">
+        <v>200</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="12">
+        <v>200</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="12">
+        <v>200</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="12">
+        <v>200</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D0165883-B711-4AE6-B3D2-78B807C6FEA0}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{137FBA2D-574D-4B81-80EA-917919005AE4}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{0BC74270-8F34-4D4E-B265-83C3F4046B28}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{49F47022-8407-4DC7-9878-C0EBB909F052}"/>
+    <hyperlink ref="H3" r:id="rId5" xr:uid="{51E5E6E3-F3E7-4AAF-A1E9-16B2C2EBC272}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{EC92CBA8-9711-476A-8514-A46970AB4330}"/>
+    <hyperlink ref="G4" r:id="rId7" xr:uid="{9A65B6E6-CE9F-46BD-A8CB-5883912994BF}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{DA0F76FF-E012-45EB-BDEC-0702B556D5D6}"/>
+    <hyperlink ref="G5" r:id="rId9" xr:uid="{B44C7F1E-5837-4FBE-A45D-CE69E94A8743}"/>
+    <hyperlink ref="E6" r:id="rId10" xr:uid="{48486199-52A3-4233-B9B3-FCF585AD9015}"/>
+    <hyperlink ref="G6" r:id="rId11" xr:uid="{E416AE9F-9A48-4AC3-B097-BE2D814BB3ED}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{37215E58-29AD-443E-A4E9-484E5B03594F}"/>
+    <hyperlink ref="G7" r:id="rId13" xr:uid="{D57B77ED-066E-4D97-AECD-EBFF50C0E174}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B016B5-A424-43E2-9D21-B2706CFF155C}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="12">
+        <v>2000</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2000</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1000</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{6FE1A839-3A66-40C7-9D47-E837FA302749}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{8A7CA079-BFEC-49EB-83DB-DFA7EAC9D464}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{EABF28BA-3446-41C0-A651-84262A2A5CB4}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{50A935C9-6BD0-41D8-AF96-33ECC98CFCC2}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{5C0858DE-B83F-44B8-B658-10382FDE2DB0}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{EA14F21F-B7F6-49B9-A1BF-953234F55846}"/>
+    <hyperlink ref="G4" r:id="rId7" xr:uid="{906B007D-FB38-4944-83F9-55524AFCE3C3}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{B086BF29-0CA6-41D0-AFCE-7673ED72DDAE}"/>
+    <hyperlink ref="G5" r:id="rId9" xr:uid="{FF0A2560-C670-4D35-9AE8-D4B3471441BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update app, Excel, and HTML templates
</commit_message>
<xml_diff>
--- a/storage.xlsx
+++ b/storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarav\Projects\coinsora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BFE764-1294-49AC-B87B-7AE3C9319D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F51739-8B73-405B-8C15-F86EE1EB2964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A4295153-D957-4117-8BC1-D264311D4EE7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A4295153-D957-4117-8BC1-D264311D4EE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Old Coin Showcase" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="203">
   <si>
     <t>ID</t>
   </si>
@@ -389,9 +389,6 @@
     <t>This commemorative coin was issued in 2003 to celebrate the 150th anniversary of Indian Railways, which was established in 1853. The reverse features "Bholu the Guard," the elephant mascot of Indian Railways, holding a signal lamp, along with inscriptions "Railways," "150 Glorious Years," and "Bholu The Guard" (in both English and Hindi), and the year 2003. The obverse shows the Lion Capital of Ashoka above the denomination "2 Rupees" in Hindi and English. The coin is copper-nickel, weighs about 6.05 grams, and is 26.5 mm in diameter, with an 11-sided (hendecagonal) shape. Issued by all four Indian mints: Mumbai, Hyderabad, Kolkata, and Noida.</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760868418/20251019_093637_kjqlgh.jpg</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760868417/20251019_093702_prnuyv.jpg</t>
   </si>
   <si>
@@ -401,21 +398,12 @@
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760868414/20251019_093734_ewmk0h.jpg</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869070/20251019_094124_banlty.jpg</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869048/20251019_094042_q5dniz.jpg</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869045/20251019_094227_rxgbjf.jpg</t>
   </si>
   <si>
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869043/20251019_094220_nhwy4d.jpg</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869351/20251019_094430_hfoocx.jpg</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869350/20251019_094439_oflxqf.jpg</t>
   </si>
   <si>
@@ -425,9 +413,6 @@
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869359/20251019_094454_iownsx.jpg</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869577/20251019_094721_xeenqd.jpg</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869577/20251019_094728_isfvsc.jpg</t>
   </si>
   <si>
@@ -437,21 +422,6 @@
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869572/20251019_094740_ekzmxy.jpg</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869792/20251019_094840_qzmuyn.jpg</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869792/20251019_094847_qbclhe.jpg</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869793/20251019_094857_kg8idr.jpg</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869793/20251019_094901_pkgod6.jpg</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869851/20251019_095229_paoblv.jpg</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869853/20251019_095243_l5eezq.jpg</t>
   </si>
   <si>
@@ -461,9 +431,6 @@
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869855/20251019_095247_gll09g.jpg</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869916/20251019_095419_jw0lfx.jpg</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760869915/20251019_095428_tiff9l.jpg</t>
   </si>
   <si>
@@ -594,6 +561,90 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760871855/20251019_101711_eipmi9.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760879219/20251019_093637_kjqlgh.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760879384/20251019_094124_banlty.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760879496/20251019_094042_q5dniz.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760879774/20251019_094430_hfoocx.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760880005/20251019_094721_xeenqd.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760880207/20251019_094847_qbclhe.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760876499/20251019_094840_qzmuyn.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760876560/20251019_094901_pkgod6.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760876638/20251019_094857_kg8idr.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760876681/20251019_095229_paoblv.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dzluvgbia/image/upload/v1760877163/20251019_095419_jw0lfx.jpg</t>
+  </si>
+  <si>
+    <t>LEADER-COIN-002</t>
+  </si>
+  <si>
+    <t>LEADER-COIN-003</t>
+  </si>
+  <si>
+    <t>LEADER-COIN-004</t>
+  </si>
+  <si>
+    <t>LEADER-COIN-005</t>
+  </si>
+  <si>
+    <t>LEADER-COIN-006</t>
+  </si>
+  <si>
+    <t>LEADER-COIN-007</t>
+  </si>
+  <si>
+    <t>LEADER-COIN-008</t>
+  </si>
+  <si>
+    <t>LEADER-COIN-009</t>
+  </si>
+  <si>
+    <t>LEADER-COIN-010</t>
+  </si>
+  <si>
+    <t>LEADER-COIN-011</t>
+  </si>
+  <si>
+    <t>NOTE-001</t>
+  </si>
+  <si>
+    <t>NOTE-002</t>
+  </si>
+  <si>
+    <t>NOTE-003</t>
+  </si>
+  <si>
+    <t>NOTE-004</t>
+  </si>
+  <si>
+    <t>NOTE-005</t>
+  </si>
+  <si>
+    <t>NOTE-006</t>
+  </si>
+  <si>
+    <t>NOTE-007</t>
   </si>
 </sst>
 </file>
@@ -658,7 +709,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -669,8 +720,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -989,7 +1038,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1414,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19989FF-8C56-43F6-A462-200A6BE109D0}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1504,29 +1553,32 @@
       <c r="B3" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>186</v>
+      </c>
       <c r="D3">
         <v>2000</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>99</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.35">
@@ -1536,29 +1588,32 @@
       <c r="B4" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="D4">
         <v>5000</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>101</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.35">
@@ -1568,29 +1623,32 @@
       <c r="B5" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="D5">
         <v>2000</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>102</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.35">
@@ -1600,29 +1658,32 @@
       <c r="B6" s="3" t="s">
         <v>103</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="D6">
         <v>5000</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>104</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.35">
@@ -1632,29 +1693,32 @@
       <c r="B7" s="3" t="s">
         <v>105</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="D7">
         <v>20000</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>108</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.35">
@@ -1664,29 +1728,32 @@
       <c r="B8" s="3" t="s">
         <v>106</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>191</v>
+      </c>
       <c r="D8">
         <v>10000</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>107</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.35">
@@ -1696,29 +1763,32 @@
       <c r="B9" s="3" t="s">
         <v>109</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="D9">
         <v>20000</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>110</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.35">
@@ -1728,29 +1798,32 @@
       <c r="B10" s="3" t="s">
         <v>111</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="D10">
         <v>2000</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>112</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.35">
@@ -1760,29 +1833,32 @@
       <c r="B11" s="3" t="s">
         <v>113</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="D11">
         <v>5000</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>114</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.35">
@@ -1792,32 +1868,36 @@
       <c r="B12" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="D12">
         <v>1000</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>116</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{FD7ABBB0-646E-42E5-A29F-BE8814F05A92}"/>
     <hyperlink ref="G2" r:id="rId2" xr:uid="{FFF5C0AA-ADCB-4649-8E7B-18060440BBAA}"/>
@@ -1883,20 +1963,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7256E16C-20E7-4C56-A2FE-7502923055E2}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="6"/>
-    <col min="3" max="3" width="15.88671875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="6"/>
-    <col min="5" max="5" width="18.88671875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="14.6640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1935,266 +2011,288 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="6">
+      <c r="C2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2">
         <v>70000</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="K2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3">
+        <v>10000</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="K3" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4">
         <v>10000</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="I4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="6">
-        <v>10000</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="6">
+      <c r="C5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5">
         <v>10000</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>145</v>
+        <v>179</v>
+      </c>
+      <c r="F5" t="s">
+        <v>134</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>129</v>
+        <v>179</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>90</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="6">
+      <c r="C6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6">
         <v>5000</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>145</v>
+        <v>180</v>
+      </c>
+      <c r="F6" t="s">
+        <v>134</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>92</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>136</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="6">
+      <c r="C7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7">
         <v>200000</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>145</v>
+        <v>184</v>
+      </c>
+      <c r="F7" t="s">
+        <v>134</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>94</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="6">
+      <c r="C8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D8">
         <v>5000</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>145</v>
+        <v>185</v>
+      </c>
+      <c r="F8" t="s">
+        <v>134</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>141</v>
+        <v>185</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>96</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{34F95D33-AEA1-45E9-9111-00488F0121E4}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{6EBF151C-DDE3-49E9-BA63-CC2C59AC9F18}"/>
-    <hyperlink ref="H2" r:id="rId3" xr:uid="{B64CFC98-A5F4-4D6C-BF62-2AC0006ACEEA}"/>
-    <hyperlink ref="J2" r:id="rId4" xr:uid="{DBA95801-A5A0-44FA-8B40-1785F0DBD88E}"/>
-    <hyperlink ref="K2" r:id="rId5" xr:uid="{80353E5F-F52A-4580-B45D-82D49FBCB0BB}"/>
-    <hyperlink ref="E3" r:id="rId6" xr:uid="{F3418C03-054D-4196-B419-9E65F4827F33}"/>
-    <hyperlink ref="G3" r:id="rId7" xr:uid="{B289AC9E-1035-40C3-98A6-9D6BEF5B630E}"/>
-    <hyperlink ref="H3" r:id="rId8" xr:uid="{CC9E8CEF-1ECF-428B-A699-852EEA79FA32}"/>
-    <hyperlink ref="J3" r:id="rId9" xr:uid="{435C4EA9-AE1C-4CC8-9905-E7B5959BE78F}"/>
-    <hyperlink ref="K3" r:id="rId10" xr:uid="{53ADFE60-1D90-4EEA-91F7-6B3C33724F6F}"/>
-    <hyperlink ref="E4" r:id="rId11" xr:uid="{7BCA2B80-FD33-4C1D-B114-C9AB23AC1709}"/>
-    <hyperlink ref="G4" r:id="rId12" xr:uid="{6C8EADC1-7F16-43CE-87FE-BD0E3A9ED887}"/>
-    <hyperlink ref="H4" r:id="rId13" xr:uid="{FA3EBE9F-29CC-4684-9336-2B3ADF298A90}"/>
-    <hyperlink ref="J4" r:id="rId14" xr:uid="{874440EA-97F1-4D73-9CC9-64B002219966}"/>
-    <hyperlink ref="K4" r:id="rId15" xr:uid="{5160EB25-4DFA-4AF8-99E3-407BD5B8C64A}"/>
-    <hyperlink ref="E5" r:id="rId16" xr:uid="{BA190943-1D77-4D2D-8B5E-4455568D0EBC}"/>
-    <hyperlink ref="G5" r:id="rId17" xr:uid="{CCD66277-7673-48A3-9842-7FD3CEB7756C}"/>
-    <hyperlink ref="H5" r:id="rId18" xr:uid="{9ABA5046-4731-4C48-85BB-6ABB1E6AC397}"/>
-    <hyperlink ref="J5" r:id="rId19" xr:uid="{9A515923-84A7-47E0-884B-9A8B7EEAA73B}"/>
-    <hyperlink ref="K5" r:id="rId20" xr:uid="{3A8216E2-0DED-4E0F-822E-491E8570CA24}"/>
-    <hyperlink ref="E6" r:id="rId21" xr:uid="{B169A5D0-0919-4E90-B0C3-EFCEFEC910D4}"/>
-    <hyperlink ref="G6" r:id="rId22" xr:uid="{4C52A487-CFEC-49F8-BB8B-F7404BAAA05F}"/>
-    <hyperlink ref="H6" r:id="rId23" xr:uid="{46172BF0-C26A-495E-B952-32350D1F348D}"/>
-    <hyperlink ref="J6" r:id="rId24" xr:uid="{F59A6095-210F-4977-911F-A868BDB3C51D}"/>
-    <hyperlink ref="K6" r:id="rId25" xr:uid="{286AA9BF-5183-41C9-BEEB-8B3C138D59B2}"/>
-    <hyperlink ref="E7" r:id="rId26" xr:uid="{BFAE61F7-6B30-440B-8518-7FC66F0526BB}"/>
-    <hyperlink ref="G7" r:id="rId27" xr:uid="{10D2A923-0D61-410E-B13F-3E0539E8F7C3}"/>
-    <hyperlink ref="H7" r:id="rId28" xr:uid="{6E493A52-4BD3-4EB9-9349-8D0E59189A58}"/>
-    <hyperlink ref="J7" r:id="rId29" xr:uid="{C3160AAB-AF39-4AF5-809A-7F418CEC6972}"/>
-    <hyperlink ref="K7" r:id="rId30" xr:uid="{4B046FE5-42EA-48B5-BEB8-B592A8FF2512}"/>
-    <hyperlink ref="E8" r:id="rId31" xr:uid="{82BB2DED-44EA-46CC-A332-D4D5959948C5}"/>
-    <hyperlink ref="G8" r:id="rId32" xr:uid="{BAD7E8B6-8D7A-48E6-BC31-F2DC2C483E5D}"/>
-    <hyperlink ref="H8" r:id="rId33" xr:uid="{6CFD96D6-F0F3-4FB9-907F-73E0A96B7DA0}"/>
-    <hyperlink ref="J8" r:id="rId34" xr:uid="{35FE4F4E-9702-4F91-9F7C-BA12B3BA0BFE}"/>
-    <hyperlink ref="K8" r:id="rId35" xr:uid="{A6D772FA-FAF7-4AE6-AC52-49B7BBCA5AAA}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{B64CFC98-A5F4-4D6C-BF62-2AC0006ACEEA}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{DBA95801-A5A0-44FA-8B40-1785F0DBD88E}"/>
+    <hyperlink ref="K2" r:id="rId3" xr:uid="{80353E5F-F52A-4580-B45D-82D49FBCB0BB}"/>
+    <hyperlink ref="J3" r:id="rId4" xr:uid="{435C4EA9-AE1C-4CC8-9905-E7B5959BE78F}"/>
+    <hyperlink ref="K3" r:id="rId5" xr:uid="{53ADFE60-1D90-4EEA-91F7-6B3C33724F6F}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{FA3EBE9F-29CC-4684-9336-2B3ADF298A90}"/>
+    <hyperlink ref="J4" r:id="rId7" xr:uid="{874440EA-97F1-4D73-9CC9-64B002219966}"/>
+    <hyperlink ref="K4" r:id="rId8" xr:uid="{5160EB25-4DFA-4AF8-99E3-407BD5B8C64A}"/>
+    <hyperlink ref="H5" r:id="rId9" xr:uid="{9ABA5046-4731-4C48-85BB-6ABB1E6AC397}"/>
+    <hyperlink ref="J5" r:id="rId10" xr:uid="{9A515923-84A7-47E0-884B-9A8B7EEAA73B}"/>
+    <hyperlink ref="K5" r:id="rId11" xr:uid="{3A8216E2-0DED-4E0F-822E-491E8570CA24}"/>
+    <hyperlink ref="H7" r:id="rId12" xr:uid="{6E493A52-4BD3-4EB9-9349-8D0E59189A58}"/>
+    <hyperlink ref="J7" r:id="rId13" xr:uid="{C3160AAB-AF39-4AF5-809A-7F418CEC6972}"/>
+    <hyperlink ref="K7" r:id="rId14" xr:uid="{4B046FE5-42EA-48B5-BEB8-B592A8FF2512}"/>
+    <hyperlink ref="H8" r:id="rId15" xr:uid="{6CFD96D6-F0F3-4FB9-907F-73E0A96B7DA0}"/>
+    <hyperlink ref="J8" r:id="rId16" xr:uid="{35FE4F4E-9702-4F91-9F7C-BA12B3BA0BFE}"/>
+    <hyperlink ref="K8" r:id="rId17" xr:uid="{A6D772FA-FAF7-4AE6-AC52-49B7BBCA5AAA}"/>
+    <hyperlink ref="E2" r:id="rId18" xr:uid="{2ACC8460-B7BA-42BC-9FF2-E89616CB0131}"/>
+    <hyperlink ref="G2" r:id="rId19" xr:uid="{454E4E1F-2CD3-4431-AAA4-038B8FA7FBC8}"/>
+    <hyperlink ref="E3" r:id="rId20" xr:uid="{1FC25C26-A2C0-4AE6-ACB7-C0514401909A}"/>
+    <hyperlink ref="G3" r:id="rId21" xr:uid="{9D7188A0-9B0B-404C-81A1-114A92AD61BD}"/>
+    <hyperlink ref="H3" r:id="rId22" xr:uid="{AEDC3969-650A-4D48-B1ED-2C9159817C67}"/>
+    <hyperlink ref="E4" r:id="rId23" xr:uid="{A8654483-075E-48BD-8EA0-9A4AE53D5DC9}"/>
+    <hyperlink ref="G4" r:id="rId24" xr:uid="{F37DD80A-D0A8-490C-89B8-548E9500BEB3}"/>
+    <hyperlink ref="E5" r:id="rId25" xr:uid="{AAF325C0-1F10-47C7-9989-7866A3A395CF}"/>
+    <hyperlink ref="G5" r:id="rId26" xr:uid="{BC33EB00-2A8C-4771-8A5C-6A60CD398205}"/>
+    <hyperlink ref="E6" r:id="rId27" xr:uid="{634D4CE9-3B34-4449-9E98-977B1A58EB4E}"/>
+    <hyperlink ref="G6" r:id="rId28" xr:uid="{F3CD6B47-F034-435D-A437-496103A13C86}"/>
+    <hyperlink ref="H6" r:id="rId29" xr:uid="{67589472-9BE9-4F95-BAE1-F6D062C2648E}"/>
+    <hyperlink ref="J6" r:id="rId30" xr:uid="{EBFF3B82-7FCC-4A9F-B182-FDC9C93DF10B}"/>
+    <hyperlink ref="K6" r:id="rId31" xr:uid="{F4F980AA-C492-4D3F-A49B-7D39E94F957C}"/>
+    <hyperlink ref="E7" r:id="rId32" xr:uid="{94206C41-4037-4A9A-83F4-2E76CE7A440E}"/>
+    <hyperlink ref="G7" r:id="rId33" xr:uid="{CE4B945F-7DFA-4644-99DF-647714F39195}"/>
+    <hyperlink ref="E8" r:id="rId34" xr:uid="{B60492B0-1AF0-4BA9-A169-95C1EB5C464C}"/>
+    <hyperlink ref="G8" r:id="rId35" xr:uid="{E860D449-4F7A-431B-B7F3-EE5A17148825}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>